<commit_message>
Update Excel template handling to support scalar values and array definitions; enhance validation for bookings and yearMonth fields in fill-template logic.
</commit_message>
<xml_diff>
--- a/templates/commuting.xlsx
+++ b/templates/commuting.xlsx
@@ -1,41 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EFEEA4B-57BD-4E05-935C-7C09889A8A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>Test</t>
+    <t>${yearMonth}</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Empty2</t>
+  </si>
+  <si>
+    <t>Empty3</t>
+  </si>
+  <si>
+    <t>Empty4</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
   <si>
     <t>${table:bookings.day}</t>
@@ -53,11 +72,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -69,18 +85,13 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,8 +116,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -170,12 +193,32 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="13"/>
       </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="13"/>
       </bottom>
@@ -188,12 +231,34 @@
       <right style="thin">
         <color indexed="11"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="13"/>
-      </bottom>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -206,99 +271,798 @@
       <top style="thin">
         <color indexed="13"/>
       </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="11"/>
       </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="13"/>
       </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="13"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="13"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="14"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="13"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="14"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="13"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="13"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top style="thin">
+          <color indexed="13"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="13"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="11"/>
+        </left>
+        <right style="thin">
+          <color indexed="11"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9F51716-0BFF-4DEC-A3B1-1C7964D988A1}" name="Táblázat1" displayName="Táblázat1" ref="A3:G5" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A3:G4" xr:uid="{A9F51716-0BFF-4DEC-A3B1-1C7964D988A1}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8ACC5EBA-9D91-4D44-9AA6-D24080136506}" name="Day" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4C19AA70-0751-4C7F-B0E9-60A4E6F2676C}" name="Distance" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{64A6446B-4F25-4A7D-9B87-26B4CAB60E54}" name="Empty" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{86D3AAF8-8330-4396-A71F-4F7B3B069EA5}" name="Empty2" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{7560DF7A-2D9A-4D21-B41A-8D84E6E9D9ED}" name="Empty3" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{A1628EB2-13ED-4C4A-B03D-D84BBAA308BD}" name="Empty4" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{3DEB3B09-8B17-4AAC-B629-85C701CB65A5}" name="Cost" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -500,7 +1264,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -518,7 +1282,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -547,7 +1311,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -572,7 +1336,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -597,7 +1361,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -622,7 +1386,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -647,7 +1411,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -672,7 +1436,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -697,7 +1461,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -722,7 +1486,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -747,7 +1511,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,9 +1524,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -779,7 +1549,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -797,7 +1567,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -822,7 +1592,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -847,7 +1617,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -872,7 +1642,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -897,7 +1667,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -922,7 +1692,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -947,7 +1717,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +1742,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -997,7 +1767,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1022,7 +1792,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1035,9 +1805,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1051,7 +1827,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1069,7 +1845,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,7 +1874,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1899,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1148,7 +1924,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1949,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,7 +1974,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1223,7 +1999,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1248,7 +2024,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,7 +2049,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1298,7 +2074,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1311,341 +2087,113 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="27.6" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" ht="44.25" customHeight="1">
-      <c r="A3" t="s" s="6">
+    <row r="3" spans="1:7" ht="44.25" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s" s="8">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+    <row r="4" spans="1:7" ht="14.65" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" ht="14.7" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" ht="14.7" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" ht="14.7" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" ht="14.7" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" ht="14.7" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" ht="14.7" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" ht="14.7" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" ht="14.7" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" ht="14.7" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" ht="14.7" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" ht="14.7" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" ht="14.7" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" ht="14.7" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" ht="14.7" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" ht="14.7" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" ht="14.7" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" ht="14.7" customHeight="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" ht="14.7" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" ht="14.7" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" ht="14.7" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" ht="14.7" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32" ht="14.7" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" ht="14.7" customHeight="1">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="11" cm="1">
-        <f t="array" ref="G33">SUM(G3:G32)</f>
+    <row r="5" spans="1:7" ht="19.899999999999999" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14">
+        <f>SUBTOTAL(109,Táblázat1[Cost])</f>
         <v>0</v>
       </c>
     </row>
@@ -1653,10 +2201,13 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>